<commit_message>
subida de datos de respaldo dado que el original se corrompio en la ultima subida a git. Se deja constancia en la carpeta corrupt
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leasoto\Desktop\Duoc\Semestre 3\Prog_Web\Experiencia_1\Experiencia1_Arancibia_Soto_001V\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leasoto\Desktop\Experiencia1_Arancibia_Soto_001V_rescute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86556447-5656-4A38-B656-D38B5674A315}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBEE6B7B-E3C1-4D75-A52F-B77B9F20752A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39690" yWindow="6570" windowWidth="17805" windowHeight="9075" xr2:uid="{FCDE2450-F88F-495E-B1FA-0A36D45218BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{FCDE2450-F88F-495E-B1FA-0A36D45218BF}"/>
   </bookViews>
   <sheets>
     <sheet name="BitácoraExperiencia1" sheetId="2" r:id="rId1"/>
+    <sheet name="BitácoraExperiencia2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
   <si>
     <t>Equipo</t>
   </si>
@@ -106,6 +107,27 @@
   </si>
   <si>
     <t>Ultimo Commit en GIT y envio de proyecto</t>
+  </si>
+  <si>
+    <t>Crea Login Formularios html - css</t>
+  </si>
+  <si>
+    <t>crea js para mostrar  Login / Formulario</t>
+  </si>
+  <si>
+    <t>ajusta fondos y estilos para formulario</t>
+  </si>
+  <si>
+    <t>agrega funciones de una api al boton dentro de galeria</t>
+  </si>
+  <si>
+    <t>Agrega el boton de contacto via mensajeria Instantanea</t>
+  </si>
+  <si>
+    <t>prueba de api de mapa para proxima etapa del proyecto (js Generado - Requiere pago api google)</t>
+  </si>
+  <si>
+    <t>Leandro Soto</t>
   </si>
 </sst>
 </file>
@@ -149,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -158,6 +180,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -476,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3DA7284-98DD-4C9B-85C9-6827807F75AB}">
   <dimension ref="B2:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -691,4 +719,126 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9778186C-C3B5-4302-89E0-B74762DCC633}">
+  <dimension ref="B2:D12"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="105.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="2">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="2">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="2">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="2">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>